<commit_message>
EDUCATION trend work and other minor edits
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/Age Group Standard and US Standard 2000 Population.xlsx
+++ b/myCBD/myInfo/Age Group Standard and US Standard 2000 Population.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="24915" windowHeight="12090"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="24915" windowHeight="12090" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="references" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="dataEducation" sheetId="4" r:id="rId2"/>
+    <sheet name="references" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>https://www.cdc.gov/nchs/data/statnt/statnt20.pdf</t>
   </si>
@@ -391,13 +392,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -527,6 +528,79 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="52.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>34</v>
+      </c>
+      <c r="C2">
+        <v>37233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>44</v>
+      </c>
+      <c r="C3">
+        <v>44659</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <v>64</v>
+      </c>
+      <c r="C4">
+        <v>60991</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>65</v>
+      </c>
+      <c r="B5">
+        <v>999</v>
+      </c>
+      <c r="C5">
+        <v>34710</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -587,7 +661,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
additional age groupings to age info file; and edits to technical doc
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/Age Group Standard and US Standard 2000 Population.xlsx
+++ b/myCBD/myInfo/Age Group Standard and US Standard 2000 Population.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="24915" windowHeight="12090" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="24915" windowHeight="12090" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="dataEducation" sheetId="4" r:id="rId2"/>
     <sheet name="references" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="teenAge" sheetId="3" r:id="rId4"/>
+    <sheet name="drinkAge" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>https://www.cdc.gov/nchs/data/statnt/statnt20.pdf</t>
   </si>
@@ -393,7 +394,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -663,12 +664,95 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>65</v>
+      </c>
+      <c r="B4">
+        <v>999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>65</v>
+      </c>
+      <c r="B4">
+        <v>999</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
multiple 2019 update and cleaning steps to publish
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/Age Group Standard and US Standard 2000 Population.xlsx
+++ b/myCBD/myInfo/Age Group Standard and US Standard 2000 Population.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0.CBD\myCBD\myInfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\CCB\CCB Project\0.CCB\myCBD\myInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85ACF694-BE95-4C30-94D6-35889086BD2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="24915" windowHeight="12090"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -18,12 +19,22 @@
     <sheet name="teenAge" sheetId="3" r:id="rId4"/>
     <sheet name="drinkAge" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>https://www.cdc.gov/nchs/data/statnt/statnt20.pdf</t>
   </si>
@@ -77,12 +88,18 @@
   </si>
   <si>
     <t>85+</t>
+  </si>
+  <si>
+    <t>45 - 64</t>
+  </si>
+  <si>
+    <t>65 - 999</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,6 +240,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -258,6 +292,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -433,11 +484,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,11 +656,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,7 +668,7 @@
     <col min="3" max="3" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -627,8 +678,11 @@
       <c r="C1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>25</v>
       </c>
@@ -638,8 +692,11 @@
       <c r="C2">
         <v>37233</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>35</v>
       </c>
@@ -649,8 +706,11 @@
       <c r="C3">
         <v>44659</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>45</v>
       </c>
@@ -660,8 +720,11 @@
       <c r="C4">
         <v>60991</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>65</v>
       </c>
@@ -670,6 +733,9 @@
       </c>
       <c r="C5">
         <v>34710</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -678,7 +744,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -729,9 +795,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A1" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A1" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -739,7 +805,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -787,7 +853,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>